<commit_message>
Fix metadata block parser when Excel first cell is blank (None)
</commit_message>
<xml_diff>
--- a/pdtable/test/readers/input/foo.xlsx
+++ b/pdtable/test/readers/input/foo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeaco\repos\pdtable\tables\readers\tests\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeaco\repos\pdtable\pdtable\test\readers\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E0D3F-3E84-4E2C-ACB2-4691C3BB5B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01B0DF2-1B41-41B9-9615-99C6570B924A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>all</t>
   </si>
@@ -91,6 +91,27 @@
   </si>
   <si>
     <t>FaLsE</t>
+  </si>
+  <si>
+    <t>author:</t>
+  </si>
+  <si>
+    <t>XYODA</t>
+  </si>
+  <si>
+    <t>purpose:</t>
+  </si>
+  <si>
+    <t>Save the galaxy</t>
+  </si>
+  <si>
+    <t>War and Peace</t>
+  </si>
+  <si>
+    <t>***read_this_summer</t>
+  </si>
+  <si>
+    <t>Crime and Punishment</t>
   </si>
 </sst>
 </file>
@@ -442,137 +463,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B433973-3070-4A41-BCCD-AE6DD659FC75}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B23" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>